<commit_message>
Tasks：A1, A2, A3, A4, A5, A6
</commit_message>
<xml_diff>
--- a/TheCodeor /evidence.xlsx
+++ b/TheCodeor /evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29820" windowHeight="13780"/>
+    <workbookView windowWidth="29820" windowHeight="13780" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="48">
   <si>
     <t>TeamName</t>
   </si>
@@ -64,30 +64,6 @@
     <t>Community</t>
   </si>
   <si>
-    <t>team name</t>
-  </si>
-  <si>
-    <t>addr1</t>
-  </si>
-  <si>
-    <t>addr2</t>
-  </si>
-  <si>
-    <t>addr3</t>
-  </si>
-  <si>
-    <t>addr4</t>
-  </si>
-  <si>
-    <t>addr5</t>
-  </si>
-  <si>
-    <t>discord#1234</t>
-  </si>
-  <si>
-    <t>set none if no community</t>
-  </si>
-  <si>
     <t>jadefan</t>
   </si>
   <si>
@@ -118,34 +94,79 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
+    <t>ACFEF7819D40453D9464BD64ED9ACE8C63A018821F8ED900DC389304F2DCB787</t>
+  </si>
+  <si>
+    <t>jadeIrisDenomId</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
+    <t>4F530C2E783E80744C9B3063CB936E428D8A1ECDD455490DBFDDA619A720EFCF</t>
+  </si>
+  <si>
+    <t>jadeIrisNftOneId</t>
+  </si>
+  <si>
+    <t>7B650ED7D1BDB134144076B6094341226443516239CD7965D3391AA6D9E7E7DA</t>
+  </si>
+  <si>
+    <t>jadeIrisNftTwoId</t>
+  </si>
+  <si>
+    <t>48E8D02E309370A980137391C3EE4EBF9C993173C5CEB9C893E108994578CAE8</t>
+  </si>
+  <si>
+    <t>jadeIrisNftThreeId</t>
+  </si>
+  <si>
+    <t>48C770589FD3C3614892DDF8DBED1F82AA56EED135EB98B3252D4F27EAC78AF1</t>
+  </si>
+  <si>
+    <t>jadeIrisNftFourId</t>
   </si>
   <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
+    <t>ContractAdd</t>
+  </si>
+  <si>
+    <t>97A11DCD384CD3F1666817A25C09CE1049098614344AE3B4611A981C2A4C6F07</t>
+  </si>
+  <si>
+    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/jadeIrisDenomId</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>juno1f82vkl94ghtcfgz3u47cf4qt29fugz35cntle4thl47mqcwxvcmqwzrjmr</t>
+  </si>
+  <si>
+    <t>1DC48709502693E065F6D206537E99A045EAF3F73ECFDA21EDD57E8E9699021A</t>
+  </si>
+  <si>
+    <t>ibc/D1933EBEFF27681C7C9F93776582CC2D90F218CD965477E418DBA39CF8DCD84B</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>F82E8FDC3C8A8C0EBDAB300EE00553B44AE82F3599E305D81D95CE2867BC5243</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>F4583864107315A999AD78A65809202C08A2E82EAA4E3EF98F37B8292A806C44</t>
+  </si>
+  <si>
+    <t>ibc class on chain</t>
   </si>
   <si>
     <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
   </si>
   <si>
     <t>tx hash on that chain</t>
@@ -168,12 +189,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,11 +209,46 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="微软雅黑"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -202,10 +258,132 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -216,137 +394,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,7 +410,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,31 +482,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,19 +548,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,121 +584,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,7 +647,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -624,11 +667,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,21 +721,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -673,170 +731,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -845,19 +888,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1208,19 +1282,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="14.5769230769231" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.3173076923077" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.1442307692308" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1442307692308" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.1442307692308" style="24" customWidth="1"/>
     <col min="6" max="6" width="17.7211538461538" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.5769230769231" style="1" customWidth="1"/>
     <col min="8" max="8" width="36.3846153846154" style="1" customWidth="1"/>
@@ -1252,56 +1326,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" spans="1:8">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="23" customFormat="1" ht="83" customHeight="1" spans="1:8">
+      <c r="A2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="25" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="3" ht="83" customHeight="1" spans="1:8">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1329,18 +1377,18 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1368,18 +1416,18 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1407,18 +1455,18 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1446,18 +1494,18 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1485,28 +1533,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1534,28 +1582,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1583,28 +1631,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1632,28 +1680,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1681,28 +1729,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1730,28 +1778,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1767,29 +1815,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="17.8653846153846" style="1" customWidth="1"/>
+    <col min="1" max="1" width="85.2596153846154" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.0673076923077" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
+      <c r="A2" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1817,28 +1866,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1866,28 +1915,28 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1914,17 +1963,17 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1951,17 +2000,17 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1988,17 +2037,17 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2025,17 +2074,17 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2049,38 +2098,73 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.2" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="17.8653846153846" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.0096153846154" style="1" customWidth="1"/>
+    <col min="1" max="1" width="97.9134615384615" style="16" customWidth="1"/>
+    <col min="2" max="2" width="19.7019230769231" style="16" customWidth="1"/>
+    <col min="3" max="3" width="34.6057692307692" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" s="15" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" ht="16" spans="1:3">
+      <c r="A3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="4" ht="16" spans="1:3">
+      <c r="A4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" ht="16" spans="1:3">
+      <c r="A5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="2" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2094,45 +2178,53 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="17.8653846153846" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.0096153846154" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.0480769230769" style="1" customWidth="1"/>
+    <col min="2" max="2" width="103.528846153846" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1442307692308" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.4326923076923" style="1" customWidth="1"/>
+    <col min="5" max="5" width="68.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" s="12" customFormat="1" ht="17.25" customHeight="1" spans="1:5">
+      <c r="A1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" s="9" customFormat="1" ht="18" customHeight="1" spans="1:5">
+      <c r="A2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="11" t="s">
         <v>33</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2149,42 +2241,43 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="17.8653846153846" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.0096153846154" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.4326923076923" style="1" customWidth="1"/>
+    <col min="1" max="1" width="54.4807692307692" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7884615384615" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1826923076923" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.3076923076923" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" s="9" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2201,42 +2294,43 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="17.8653846153846" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.0096153846154" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.4326923076923" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.9615384615385" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.5288461538462" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.8846153846154" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1538461538462" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" s="7" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>33</v>
+      <c r="D2" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2253,43 +2347,43 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.8653846153846" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.0096153846154" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.2884615384615" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.4326923076923" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.4134615384615" style="1" customWidth="1"/>
+    <col min="2" max="2" width="59.7692307692308" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.3557692307692" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.0480769230769" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" s="4" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2317,18 +2411,18 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2356,18 +2450,18 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix  error a3 a5 a6 ,add b1 b2
</commit_message>
<xml_diff>
--- a/TheCodeor /evidence.xlsx
+++ b/TheCodeor /evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29820" windowHeight="13780" firstSheet="12" activeTab="20"/>
+    <workbookView windowWidth="29820" windowHeight="13780" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="96">
   <si>
     <t>TeamName</t>
   </si>
@@ -130,21 +130,15 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>ContractAdd</t>
-  </si>
-  <si>
     <t>97A11DCD384CD3F1666817A25C09CE1049098614344AE3B4611A981C2A4C6F07</t>
   </si>
   <si>
-    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/jadeIrisDenomId</t>
+    <t>juno1f82vkl94ghtcfgz3u47cf4qt29fugz35cntle4thl47mqcwxvcmqwzrjmr</t>
   </si>
   <si>
     <t>uni-6</t>
   </si>
   <si>
-    <t>juno1f82vkl94ghtcfgz3u47cf4qt29fugz35cntle4thl47mqcwxvcmqwzrjmr</t>
-  </si>
-  <si>
     <t>1DC48709502693E065F6D206537E99A045EAF3F73ECFDA21EDD57E8E9699021A</t>
   </si>
   <si>
@@ -157,51 +151,51 @@
     <t>F82E8FDC3C8A8C0EBDAB300EE00553B44AE82F3599E305D81D95CE2867BC5243</t>
   </si>
   <si>
+    <t>F4583864107315A999AD78A65809202C08A2E82EAA4E3EF98F37B8292A806C44</t>
+  </si>
+  <si>
+    <t>ibc/D9C01597BD1B8721CFEE4F99CAEB73FF064FE5C8A74F538151B2260FDBEF04DB</t>
+  </si>
+  <si>
+    <t>jadefanA7NFTId</t>
+  </si>
+  <si>
+    <t>ibc/2C6B1232A8C94D5B272C7892ED17CFC2A0B3D510A6D856579C9A16532678580C</t>
+  </si>
+  <si>
+    <t>jadefanA8NFTId</t>
+  </si>
+  <si>
+    <t>ibc/FD7ED146C8BB20786D430400AF9D3F120714923CC39386C5C52CD7B5E954B556</t>
+  </si>
+  <si>
+    <t>jadefanA9NFTId</t>
+  </si>
+  <si>
+    <t>ibc/7A8F58D0676FADF5F2FB62712E989A1F55B6E54A6D70C145546D768520B02549</t>
+  </si>
+  <si>
+    <t>jadefanA10NFTId</t>
+  </si>
+  <si>
+    <t>ibc/527D5F2FBB1EB1BAAB23B54CF821D58F4FE3C992F25CB2482B78F6C41ECF5D7E</t>
+  </si>
+  <si>
+    <t>jadefanA11NFTId</t>
+  </si>
+  <si>
+    <t>ibc/36A2AE11F54055D1869F656516419199231B745A971867C320D7476D0B1BAC21</t>
+  </si>
+  <si>
+    <t>jadefanA12NFTId</t>
+  </si>
+  <si>
+    <t>020C9D258C9C1492A1EA5A42584F846B54E26FA6F754C99DAAC60125166E664E</t>
+  </si>
+  <si>
     <t>gon-irishub-1</t>
   </si>
   <si>
-    <t>F4583864107315A999AD78A65809202C08A2E82EAA4E3EF98F37B8292A806C44</t>
-  </si>
-  <si>
-    <t>ibc/D9C01597BD1B8721CFEE4F99CAEB73FF064FE5C8A74F538151B2260FDBEF04DB</t>
-  </si>
-  <si>
-    <t>jadefanA7NFTId</t>
-  </si>
-  <si>
-    <t>ibc/2C6B1232A8C94D5B272C7892ED17CFC2A0B3D510A6D856579C9A16532678580C</t>
-  </si>
-  <si>
-    <t>jadefanA8NFTId</t>
-  </si>
-  <si>
-    <t>ibc/FD7ED146C8BB20786D430400AF9D3F120714923CC39386C5C52CD7B5E954B556</t>
-  </si>
-  <si>
-    <t>jadefanA9NFTId</t>
-  </si>
-  <si>
-    <t>ibc/7A8F58D0676FADF5F2FB62712E989A1F55B6E54A6D70C145546D768520B02549</t>
-  </si>
-  <si>
-    <t>jadefanA10NFTId</t>
-  </si>
-  <si>
-    <t>ibc/527D5F2FBB1EB1BAAB23B54CF821D58F4FE3C992F25CB2482B78F6C41ECF5D7E</t>
-  </si>
-  <si>
-    <t>jadefanA11NFTId</t>
-  </si>
-  <si>
-    <t>ibc/36A2AE11F54055D1869F656516419199231B745A971867C320D7476D0B1BAC21</t>
-  </si>
-  <si>
-    <t>jadefanA12NFTId</t>
-  </si>
-  <si>
-    <t>020C9D258C9C1492A1EA5A42584F846B54E26FA6F754C99DAAC60125166E664E</t>
-  </si>
-  <si>
     <t>A310CA0094A52381B86A16B0895CDE050C6EC239E2036F1E7F4C46893D058F13</t>
   </si>
   <si>
@@ -314,6 +308,18 @@
   </si>
   <si>
     <t>40ED3D6436D3BD4432B9F031D3E3C00A38BA52C5FBEA178DAD88739BF9CB8788</t>
+  </si>
+  <si>
+    <t>E51FC2FA39BFEC64E76F54F6557646745E7F7B777A197B263FB024E14105A84E</t>
+  </si>
+  <si>
+    <t>1A41E90CFBE61930A22C83DDE2976E0821A4379F44175090F3743366C2A8C1D4</t>
+  </si>
+  <si>
+    <t>0FAEBC818F5FE3D61A7AE265B613C55C9E54C75E5771B346542530F7B611A329</t>
+  </si>
+  <si>
+    <t>E8A705BCFC7207F0F44619B5F510C1E91DD2DACAD121E9AFCFFB0F88C108519C</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -327,12 +333,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +353,32 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF24292F"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1A202C"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -360,13 +392,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF24292F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -421,9 +446,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="微软雅黑"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -448,6 +478,21 @@
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -457,10 +502,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -473,6 +519,74 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -496,23 +610,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -525,74 +623,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -615,187 +645,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,6 +887,24 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -864,16 +912,42 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -893,146 +967,102 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1041,65 +1071,65 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,101 +1138,106 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1565,7 +1600,7 @@
     <col min="2" max="2" width="21.3173076923077" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.1442307692308" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1442307692308" style="45" customWidth="1"/>
+    <col min="5" max="5" width="18.1442307692308" style="48" customWidth="1"/>
     <col min="6" max="6" width="17.7211538461538" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.5769230769231" style="1" customWidth="1"/>
     <col min="8" max="8" width="36.3846153846154" style="1" customWidth="1"/>
@@ -1597,29 +1632,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="44" customFormat="1" ht="83" customHeight="1" spans="1:8">
-      <c r="A2" s="46" t="s">
+    <row r="2" s="47" customFormat="1" ht="83" customHeight="1" spans="1:8">
+      <c r="A2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="49" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1658,14 +1693,14 @@
     </row>
     <row r="2" customFormat="1" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="21"/>
+      <c r="A3" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1701,14 +1736,14 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" ht="17.6" spans="1:1">
-      <c r="A3" s="7"/>
+      <c r="A3" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1743,10 +1778,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1782,14 +1817,14 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="17.6" spans="1:1">
-      <c r="A3" s="7"/>
+      <c r="A3" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1825,45 +1860,45 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" s="15" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A2" s="16" t="s">
+    <row r="2" s="20" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" s="20" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" s="15" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A3" s="17" t="s">
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" s="20" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A4" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" s="20" customFormat="1" ht="17" spans="1:3">
+      <c r="A5" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" s="15" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A4" s="17" t="s">
+      <c r="B5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="15"/>
+    </row>
+    <row r="6" ht="19" customHeight="1" spans="1:1">
+      <c r="A6" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" s="15" customFormat="1" ht="17" spans="1:3">
-      <c r="A5" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" ht="19" customHeight="1" spans="1:1">
-      <c r="A6" s="19" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1899,48 +1934,48 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" s="9" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A2" s="10" t="s">
+    <row r="2" s="16" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" s="16" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" s="16" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A4" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A3" s="12" t="s">
+      <c r="B4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A4" s="12" t="s">
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" s="16" customFormat="1" ht="14" spans="1:3">
+      <c r="A5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="11"/>
-    </row>
-    <row r="5" s="9" customFormat="1" ht="14" spans="1:3">
-      <c r="A5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" s="9" customFormat="1" ht="13.6" spans="1:3">
-      <c r="A6" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" s="16" customFormat="1" ht="13.6" spans="1:3">
+      <c r="A6" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1978,39 +2013,39 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" ht="17" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2048,43 +2083,39 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" ht="17" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2120,52 +2151,52 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>70</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>55</v>
+        <v>71</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>72</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" ht="17" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>55</v>
+        <v>73</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" ht="17.6" spans="1:1">
-      <c r="A6" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" ht="17" spans="3:3">
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" ht="17" spans="3:3">
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" ht="17" spans="3:3">
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" ht="17" spans="3:3">
-      <c r="C14" s="4"/>
+      <c r="A6" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3">
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="3:3">
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="3:3">
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" s="11"/>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" s="1"/>
@@ -2204,38 +2235,38 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>74</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
+        <v>76</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" ht="17" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>77</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" ht="17.6" spans="1:1">
-      <c r="A7" s="7"/>
+      <c r="A7" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2269,10 +2300,10 @@
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="38" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2290,7 +2321,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="1"/>
@@ -2310,50 +2341,50 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>78</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>79</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>80</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" ht="17" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>81</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" ht="17" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>82</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" ht="17" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>55</v>
+        <v>83</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2369,7 +2400,7 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2391,62 +2422,61 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>84</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
+      <c r="A3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" ht="17" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>87</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" ht="17" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>88</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" ht="17" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>89</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" ht="17.6" spans="1:1">
-      <c r="A8" s="7"/>
+      <c r="A8" s="14"/>
     </row>
     <row r="10" ht="17.6" spans="1:1">
-      <c r="A10" s="7"/>
+      <c r="A10" s="14"/>
     </row>
     <row r="17" ht="17.6" spans="1:1">
-      <c r="A17" s="7"/>
+      <c r="A17" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2459,15 +2489,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="12.4326923076923" style="1" customWidth="1"/>
+    <col min="1" max="1" width="86.7019230769231" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
@@ -2475,15 +2505,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="16.4" customHeight="1" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>93</v>
-      </c>
+    <row r="2" s="6" customFormat="1" ht="16.4" customHeight="1" spans="1:1">
+      <c r="A2" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" s="6" customFormat="1" ht="17.25" customHeight="1" spans="1:1">
+      <c r="A3" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" ht="17.6" spans="1:1">
+      <c r="A8" s="9"/>
+    </row>
+    <row r="10" ht="17.6" spans="1:1">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2496,15 +2535,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="$A8:$XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="12.4326923076923" style="1" customWidth="1"/>
+    <col min="1" max="1" width="111.692307692308" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
@@ -2522,6 +2561,15 @@
         <v>93</v>
       </c>
     </row>
+    <row r="8" ht="24" hidden="1" customHeight="1"/>
+    <row r="9" ht="17.6" hidden="1" spans="1:1">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" hidden="1" spans="1:1">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" hidden="1"/>
+    <row r="12" hidden="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2551,12 +2599,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2588,12 +2636,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2615,64 +2663,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.2" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="97.9134615384615" style="39" customWidth="1"/>
-    <col min="2" max="2" width="19.7019230769231" style="39" customWidth="1"/>
-    <col min="3" max="3" width="34.6057692307692" style="39" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="38"/>
+    <col min="1" max="1" width="97.9134615384615" style="42" customWidth="1"/>
+    <col min="2" max="2" width="19.7019230769231" style="42" customWidth="1"/>
+    <col min="3" max="3" width="34.6057692307692" style="42" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="41"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" s="38" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
-      <c r="A2" s="38" t="s">
+    <row r="2" s="41" customFormat="1" ht="17.25" customHeight="1" spans="1:3">
+      <c r="A2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="44" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" ht="16" spans="1:3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="44" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" ht="16" spans="1:3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="44" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" ht="16" spans="1:3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="44" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2690,51 +2738,46 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E1" sqref="E1:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="28.0480769230769" style="1" customWidth="1"/>
-    <col min="2" max="2" width="103.528846153846" style="1" customWidth="1"/>
+    <col min="1" max="1" width="84.4615384615385" style="1" customWidth="1"/>
+    <col min="2" max="2" width="72.1153846153846" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.1442307692308" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.4326923076923" style="1" customWidth="1"/>
     <col min="5" max="5" width="68.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="30" customFormat="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="37" t="s">
+    <row r="1" s="33" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="30" t="s">
+    </row>
+    <row r="2" s="37" customFormat="1" ht="18" customHeight="1" spans="1:5">
+      <c r="A2" s="38" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" s="34" customFormat="1" ht="18" customHeight="1" spans="1:5">
-      <c r="A2" s="35" t="s">
+      <c r="B2" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="C2" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>34</v>
-      </c>
+      <c r="E2" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2775,18 +2818,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" s="34" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A2" s="35" t="s">
+    <row r="2" s="37" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A2" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2803,13 +2846,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="25.9615384615385" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.5288461538462" style="1" customWidth="1"/>
+    <col min="1" max="1" width="52.8846153846154" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.8846153846154" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.1538461538462" style="1" customWidth="1"/>
   </cols>
@@ -2828,18 +2871,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" s="30" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A2" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="31" t="s">
+    <row r="2" s="33" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A2" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2855,8 +2898,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2881,18 +2924,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" s="30" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
-      <c r="A2" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="31" t="s">
+    <row r="2" s="33" customFormat="1" ht="17.25" customHeight="1" spans="1:4">
+      <c r="A2" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>39</v>
+      <c r="D2" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2914,31 +2957,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="64.9038461538462" style="25" customWidth="1"/>
-    <col min="2" max="2" width="21.9519230769231" style="25" customWidth="1"/>
-    <col min="3" max="3" width="13.4615384615385" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="24"/>
+    <col min="1" max="1" width="64.9038461538462" style="28" customWidth="1"/>
+    <col min="2" max="2" width="21.9519230769231" style="28" customWidth="1"/>
+    <col min="3" max="3" width="13.4615384615385" style="28" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="1" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+    <row r="1" s="28" customFormat="1" ht="17.25" customHeight="1" spans="1:2">
+      <c r="A1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="A2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="32"/>
     </row>
     <row r="11" ht="17.6" spans="1:1">
-      <c r="A11" s="7"/>
+      <c r="A11" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2971,22 +3014,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" s="22" customFormat="1" ht="24" customHeight="1" spans="1:2">
-      <c r="A2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>44</v>
+    <row r="2" s="26" customFormat="1" ht="24" customHeight="1" spans="1:2">
+      <c r="A2" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="21"/>
+      <c r="A3" s="25"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="21"/>
+      <c r="A4" s="25"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="21"/>
+      <c r="A5" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>